<commit_message>
added report so far
</commit_message>
<xml_diff>
--- a/Corpus/Preperation/Risk Analysis.xlsx
+++ b/Corpus/Preperation/Risk Analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Elly/Corpus/Corpus/Preperation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Otto\Desktop\STAGE3\PROJECT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A891E5F-8EB8-794C-9B82-BF614EA6B31A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1FFCCBE-4C67-41D3-B184-2A55E87802EB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="460" windowWidth="25040" windowHeight="13420" xr2:uid="{021716BD-D997-FD4F-AA2A-31CA21A41B86}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{021716BD-D997-FD4F-AA2A-31CA21A41B86}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,17 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>Risk Analysis</t>
   </si>
@@ -87,13 +82,52 @@
   </si>
   <si>
     <t>9 then 6</t>
+  </si>
+  <si>
+    <t>&lt;5 = Low</t>
+  </si>
+  <si>
+    <t>6-10 = Medium</t>
+  </si>
+  <si>
+    <t>&gt;10 = High</t>
+  </si>
+  <si>
+    <t>Dedicate enough time in advance to avoid it</t>
+  </si>
+  <si>
+    <t>Insufficient time for QA testing</t>
+  </si>
+  <si>
+    <t>Lack of/no communication</t>
+  </si>
+  <si>
+    <t>Have weekly meetings where we update eachother and discuss next steps/progression</t>
+  </si>
+  <si>
+    <t>Google charging for Firebase services</t>
+  </si>
+  <si>
+    <t>Have alternative plans if we need to hop services</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>Mistake on version control leads to loss of code</t>
+  </si>
+  <si>
+    <t>Make sure everyone is familiar and competent with github processes before we start. Following tutorials beforehand and maybe having a dummy repo to practice on.</t>
+  </si>
+  <si>
+    <t>high</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -115,8 +149,29 @@
       <name val="Cambria"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -131,12 +186,21 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -159,20 +223,14 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thick">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -182,13 +240,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -196,11 +247,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="2" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -513,140 +586,231 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27DE9BD5-D54F-8547-962A-F1E1733D9B19}">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.33203125" customWidth="1"/>
-    <col min="2" max="2" width="41.83203125" customWidth="1"/>
+    <col min="1" max="1" width="39.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.25" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1640625" customWidth="1"/>
+    <col min="4" max="4" width="17.875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="25.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="8" t="s">
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="15"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="6">
         <v>3</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="68" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="63" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="6">
         <v>3</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="6">
         <v>2</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="6">
         <v>6</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="6">
         <v>5</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="6">
         <v>2</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="6">
         <v>10</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="6">
         <v>5</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="6">
         <v>2</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="6">
         <v>10</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="12" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:6" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="5"/>
+    <row r="10" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="6">
+        <v>3</v>
+      </c>
+      <c r="D10" s="6">
+        <v>2</v>
+      </c>
+      <c r="E10" s="6">
+        <v>6</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="13">
+        <v>4</v>
+      </c>
+      <c r="D11" s="13">
+        <v>2</v>
+      </c>
+      <c r="E11" s="13">
+        <v>8</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="6">
+        <v>5</v>
+      </c>
+      <c r="D12" s="6">
+        <v>1</v>
+      </c>
+      <c r="E12" s="6">
+        <v>5</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="13">
+        <v>5</v>
+      </c>
+      <c r="D13" s="13">
+        <v>2</v>
+      </c>
+      <c r="E13" s="13">
+        <v>10</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="11" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>